<commit_message>
fixed  xls files execution
</commit_message>
<xml_diff>
--- a/Spr/xls_forms/FB.xlsx
+++ b/Spr/xls_forms/FB.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" checkCompatibility="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="225" yWindow="375" windowWidth="26085" windowHeight="11610"/>
+    <workbookView xWindow="228" yWindow="372" windowWidth="26088" windowHeight="11616"/>
   </bookViews>
   <sheets>
-    <sheet name="Контроль Форма22" sheetId="7" r:id="rId1"/>
+    <sheet name="Контроль_Форма22" sheetId="7" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="Exp">#REF!</definedName>
     <definedName name="ExpB_24_04_2015_11_47">#REF!</definedName>
     <definedName name="ExpFormaB_Work">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -663,7 +663,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1284,6 +1284,72 @@
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1307,72 +1373,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1467,6 +1467,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1514,7 +1517,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1549,7 +1552,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1767,445 +1770,445 @@
       <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="48.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="72" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="72" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A1" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="86" t="s">
+      <c r="B1" s="68" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="68" t="s">
         <v>151</v>
       </c>
-      <c r="D1" s="86" t="s">
+      <c r="D1" s="68" t="s">
         <v>152</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="86" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="86" t="s">
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="X1" s="93"/>
-      <c r="Y1" s="93"/>
-      <c r="Z1" s="93"/>
-      <c r="AA1" s="93"/>
-      <c r="AB1" s="93"/>
-      <c r="AC1" s="93"/>
-      <c r="AD1" s="93"/>
-      <c r="AE1" s="93"/>
-      <c r="AF1" s="93"/>
-      <c r="AG1" s="93"/>
-      <c r="AH1" s="93"/>
-      <c r="AI1" s="93"/>
-      <c r="AJ1" s="94" t="s">
+      <c r="X1" s="71"/>
+      <c r="Y1" s="71"/>
+      <c r="Z1" s="71"/>
+      <c r="AA1" s="71"/>
+      <c r="AB1" s="71"/>
+      <c r="AC1" s="71"/>
+      <c r="AD1" s="71"/>
+      <c r="AE1" s="71"/>
+      <c r="AF1" s="71"/>
+      <c r="AG1" s="71"/>
+      <c r="AH1" s="71"/>
+      <c r="AI1" s="71"/>
+      <c r="AJ1" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="AK1" s="93"/>
-      <c r="AL1" s="93"/>
-      <c r="AM1" s="93"/>
-      <c r="AN1" s="95" t="s">
+      <c r="AK1" s="71"/>
+      <c r="AL1" s="71"/>
+      <c r="AM1" s="71"/>
+      <c r="AN1" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="AO1" s="96"/>
-      <c r="AP1" s="96"/>
-      <c r="AQ1" s="96"/>
-      <c r="AR1" s="86" t="s">
+      <c r="AO1" s="74"/>
+      <c r="AP1" s="74"/>
+      <c r="AQ1" s="74"/>
+      <c r="AR1" s="68" t="s">
         <v>83</v>
       </c>
-      <c r="AS1" s="87"/>
-      <c r="AT1" s="87"/>
-      <c r="AU1" s="87"/>
-      <c r="AV1" s="87"/>
-      <c r="AW1" s="87"/>
-      <c r="AX1" s="87"/>
-      <c r="AY1" s="80" t="s">
+      <c r="AS1" s="69"/>
+      <c r="AT1" s="69"/>
+      <c r="AU1" s="69"/>
+      <c r="AV1" s="69"/>
+      <c r="AW1" s="69"/>
+      <c r="AX1" s="69"/>
+      <c r="AY1" s="82" t="s">
         <v>189</v>
       </c>
-      <c r="AZ1" s="80"/>
-      <c r="BA1" s="80"/>
-      <c r="BB1" s="80"/>
-      <c r="BC1" s="80"/>
-      <c r="BD1" s="80"/>
-      <c r="BE1" s="80"/>
-      <c r="BF1" s="80"/>
-      <c r="BG1" s="80"/>
-      <c r="BH1" s="80"/>
-      <c r="BI1" s="80"/>
-      <c r="BJ1" s="80"/>
-      <c r="BK1" s="80"/>
-      <c r="BL1" s="80"/>
-      <c r="BM1" s="80"/>
-      <c r="BN1" s="80"/>
-      <c r="BO1" s="80"/>
-      <c r="BP1" s="80"/>
-      <c r="BQ1" s="80"/>
-      <c r="BR1" s="80"/>
-      <c r="BS1" s="80"/>
+      <c r="AZ1" s="82"/>
+      <c r="BA1" s="82"/>
+      <c r="BB1" s="82"/>
+      <c r="BC1" s="82"/>
+      <c r="BD1" s="82"/>
+      <c r="BE1" s="82"/>
+      <c r="BF1" s="82"/>
+      <c r="BG1" s="82"/>
+      <c r="BH1" s="82"/>
+      <c r="BI1" s="82"/>
+      <c r="BJ1" s="82"/>
+      <c r="BK1" s="82"/>
+      <c r="BL1" s="82"/>
+      <c r="BM1" s="82"/>
+      <c r="BN1" s="82"/>
+      <c r="BO1" s="82"/>
+      <c r="BP1" s="82"/>
+      <c r="BQ1" s="82"/>
+      <c r="BR1" s="82"/>
+      <c r="BS1" s="82"/>
       <c r="BT1" s="1"/>
     </row>
-    <row r="2" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A2" s="97"/>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86" t="s">
+    <row r="2" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A2" s="70"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="86" t="s">
+      <c r="F2" s="68" t="s">
         <v>85</v>
       </c>
-      <c r="G2" s="86" t="s">
+      <c r="G2" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="86" t="s">
+      <c r="H2" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="86" t="s">
+      <c r="I2" s="68" t="s">
         <v>87</v>
       </c>
       <c r="J2" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="86" t="s">
+      <c r="K2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="87"/>
-      <c r="M2" s="87"/>
-      <c r="N2" s="86" t="s">
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="68" t="s">
         <v>153</v>
       </c>
-      <c r="O2" s="86" t="s">
+      <c r="O2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="87"/>
-      <c r="Q2" s="86" t="s">
+      <c r="P2" s="69"/>
+      <c r="Q2" s="68" t="s">
         <v>154</v>
       </c>
-      <c r="R2" s="86" t="s">
+      <c r="R2" s="68" t="s">
         <v>88</v>
       </c>
-      <c r="S2" s="86" t="s">
+      <c r="S2" s="68" t="s">
         <v>155</v>
       </c>
-      <c r="T2" s="86" t="s">
+      <c r="T2" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="U2" s="86" t="s">
+      <c r="U2" s="68" t="s">
         <v>90</v>
       </c>
-      <c r="V2" s="86" t="s">
+      <c r="V2" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="W2" s="86" t="s">
+      <c r="W2" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="X2" s="86" t="s">
+      <c r="X2" s="68" t="s">
         <v>91</v>
       </c>
-      <c r="Y2" s="86" t="s">
+      <c r="Y2" s="68" t="s">
         <v>92</v>
       </c>
-      <c r="Z2" s="86" t="s">
+      <c r="Z2" s="68" t="s">
         <v>157</v>
       </c>
-      <c r="AA2" s="86" t="s">
+      <c r="AA2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="87"/>
-      <c r="AD2" s="86" t="s">
+      <c r="AB2" s="69"/>
+      <c r="AC2" s="69"/>
+      <c r="AD2" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="AE2" s="92" t="s">
+      <c r="AE2" s="75" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" s="93"/>
-      <c r="AG2" s="93"/>
-      <c r="AH2" s="93"/>
-      <c r="AI2" s="93"/>
-      <c r="AJ2" s="86" t="s">
+      <c r="AF2" s="71"/>
+      <c r="AG2" s="71"/>
+      <c r="AH2" s="71"/>
+      <c r="AI2" s="71"/>
+      <c r="AJ2" s="68" t="s">
         <v>94</v>
       </c>
-      <c r="AK2" s="86" t="s">
+      <c r="AK2" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="AL2" s="87"/>
-      <c r="AM2" s="87"/>
-      <c r="AN2" s="86" t="s">
+      <c r="AL2" s="69"/>
+      <c r="AM2" s="69"/>
+      <c r="AN2" s="68" t="s">
         <v>158</v>
       </c>
-      <c r="AO2" s="86" t="s">
+      <c r="AO2" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="AP2" s="86" t="s">
+      <c r="AP2" s="68" t="s">
         <v>160</v>
       </c>
-      <c r="AQ2" s="86" t="s">
+      <c r="AQ2" s="68" t="s">
         <v>161</v>
       </c>
-      <c r="AR2" s="86" t="s">
+      <c r="AR2" s="68" t="s">
         <v>208</v>
       </c>
-      <c r="AS2" s="86" t="s">
+      <c r="AS2" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="AT2" s="87"/>
-      <c r="AU2" s="87"/>
-      <c r="AV2" s="87"/>
-      <c r="AW2" s="86" t="s">
+      <c r="AT2" s="69"/>
+      <c r="AU2" s="69"/>
+      <c r="AV2" s="69"/>
+      <c r="AW2" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="AX2" s="88" t="s">
+      <c r="AX2" s="76" t="s">
         <v>162</v>
       </c>
-      <c r="AY2" s="80"/>
-      <c r="AZ2" s="80"/>
-      <c r="BA2" s="80"/>
-      <c r="BB2" s="80"/>
-      <c r="BC2" s="80"/>
-      <c r="BD2" s="80"/>
-      <c r="BE2" s="80"/>
-      <c r="BF2" s="80"/>
-      <c r="BG2" s="80"/>
-      <c r="BH2" s="80"/>
-      <c r="BI2" s="80"/>
-      <c r="BJ2" s="80"/>
-      <c r="BK2" s="80"/>
-      <c r="BL2" s="80"/>
-      <c r="BM2" s="80"/>
-      <c r="BN2" s="80"/>
-      <c r="BO2" s="80"/>
-      <c r="BP2" s="80"/>
-      <c r="BQ2" s="80"/>
-      <c r="BR2" s="80"/>
-      <c r="BS2" s="80"/>
+      <c r="AY2" s="82"/>
+      <c r="AZ2" s="82"/>
+      <c r="BA2" s="82"/>
+      <c r="BB2" s="82"/>
+      <c r="BC2" s="82"/>
+      <c r="BD2" s="82"/>
+      <c r="BE2" s="82"/>
+      <c r="BF2" s="82"/>
+      <c r="BG2" s="82"/>
+      <c r="BH2" s="82"/>
+      <c r="BI2" s="82"/>
+      <c r="BJ2" s="82"/>
+      <c r="BK2" s="82"/>
+      <c r="BL2" s="82"/>
+      <c r="BM2" s="82"/>
+      <c r="BN2" s="82"/>
+      <c r="BO2" s="82"/>
+      <c r="BP2" s="82"/>
+      <c r="BQ2" s="82"/>
+      <c r="BR2" s="82"/>
+      <c r="BS2" s="82"/>
       <c r="BT2" s="1"/>
     </row>
-    <row r="3" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
-      <c r="B3" s="86"/>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86" t="s">
+    <row r="3" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A3" s="70"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="86" t="s">
+      <c r="K3" s="68" t="s">
         <v>163</v>
       </c>
-      <c r="L3" s="86" t="s">
+      <c r="L3" s="68" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="87"/>
-      <c r="N3" s="87"/>
-      <c r="O3" s="86" t="s">
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="68" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="86" t="s">
+      <c r="P3" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="87"/>
-      <c r="R3" s="87"/>
-      <c r="S3" s="87"/>
-      <c r="T3" s="87"/>
-      <c r="U3" s="87"/>
-      <c r="V3" s="87"/>
-      <c r="W3" s="87"/>
-      <c r="X3" s="87"/>
-      <c r="Y3" s="87"/>
-      <c r="Z3" s="87"/>
-      <c r="AA3" s="86" t="s">
+      <c r="Q3" s="69"/>
+      <c r="R3" s="69"/>
+      <c r="S3" s="69"/>
+      <c r="T3" s="69"/>
+      <c r="U3" s="69"/>
+      <c r="V3" s="69"/>
+      <c r="W3" s="69"/>
+      <c r="X3" s="69"/>
+      <c r="Y3" s="69"/>
+      <c r="Z3" s="69"/>
+      <c r="AA3" s="68" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" s="86" t="s">
+      <c r="AB3" s="68" t="s">
         <v>99</v>
       </c>
-      <c r="AC3" s="86" t="s">
+      <c r="AC3" s="68" t="s">
         <v>100</v>
       </c>
-      <c r="AD3" s="87"/>
-      <c r="AE3" s="86" t="s">
+      <c r="AD3" s="69"/>
+      <c r="AE3" s="68" t="s">
         <v>101</v>
       </c>
-      <c r="AF3" s="86" t="s">
+      <c r="AF3" s="68" t="s">
         <v>102</v>
       </c>
-      <c r="AG3" s="86" t="s">
+      <c r="AG3" s="68" t="s">
         <v>103</v>
       </c>
-      <c r="AH3" s="86" t="s">
+      <c r="AH3" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="AI3" s="86" t="s">
+      <c r="AI3" s="68" t="s">
         <v>105</v>
       </c>
-      <c r="AJ3" s="87"/>
-      <c r="AK3" s="86" t="s">
+      <c r="AJ3" s="69"/>
+      <c r="AK3" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="AL3" s="86" t="s">
+      <c r="AL3" s="68" t="s">
         <v>106</v>
       </c>
-      <c r="AM3" s="86" t="s">
+      <c r="AM3" s="68" t="s">
         <v>107</v>
       </c>
-      <c r="AN3" s="87"/>
-      <c r="AO3" s="87"/>
-      <c r="AP3" s="87"/>
-      <c r="AQ3" s="87"/>
-      <c r="AR3" s="87"/>
-      <c r="AS3" s="86" t="s">
+      <c r="AN3" s="69"/>
+      <c r="AO3" s="69"/>
+      <c r="AP3" s="69"/>
+      <c r="AQ3" s="69"/>
+      <c r="AR3" s="69"/>
+      <c r="AS3" s="68" t="s">
         <v>165</v>
       </c>
-      <c r="AT3" s="86" t="s">
+      <c r="AT3" s="68" t="s">
         <v>166</v>
       </c>
-      <c r="AU3" s="90" t="s">
+      <c r="AU3" s="78" t="s">
         <v>167</v>
       </c>
-      <c r="AV3" s="86" t="s">
+      <c r="AV3" s="68" t="s">
         <v>108</v>
       </c>
-      <c r="AW3" s="87"/>
-      <c r="AX3" s="89"/>
-      <c r="AY3" s="81"/>
-      <c r="AZ3" s="81"/>
-      <c r="BA3" s="81"/>
-      <c r="BB3" s="81"/>
-      <c r="BC3" s="81"/>
-      <c r="BD3" s="81"/>
-      <c r="BE3" s="81"/>
-      <c r="BF3" s="81"/>
-      <c r="BG3" s="81"/>
-      <c r="BH3" s="81"/>
-      <c r="BI3" s="81"/>
-      <c r="BJ3" s="81"/>
-      <c r="BK3" s="81"/>
-      <c r="BL3" s="81"/>
-      <c r="BM3" s="81"/>
-      <c r="BN3" s="81"/>
-      <c r="BO3" s="81"/>
-      <c r="BP3" s="81"/>
-      <c r="BQ3" s="81"/>
-      <c r="BR3" s="81"/>
-      <c r="BS3" s="81"/>
+      <c r="AW3" s="69"/>
+      <c r="AX3" s="77"/>
+      <c r="AY3" s="83"/>
+      <c r="AZ3" s="83"/>
+      <c r="BA3" s="83"/>
+      <c r="BB3" s="83"/>
+      <c r="BC3" s="83"/>
+      <c r="BD3" s="83"/>
+      <c r="BE3" s="83"/>
+      <c r="BF3" s="83"/>
+      <c r="BG3" s="83"/>
+      <c r="BH3" s="83"/>
+      <c r="BI3" s="83"/>
+      <c r="BJ3" s="83"/>
+      <c r="BK3" s="83"/>
+      <c r="BL3" s="83"/>
+      <c r="BM3" s="83"/>
+      <c r="BN3" s="83"/>
+      <c r="BO3" s="83"/>
+      <c r="BP3" s="83"/>
+      <c r="BQ3" s="83"/>
+      <c r="BR3" s="83"/>
+      <c r="BS3" s="83"/>
       <c r="BT3" s="1"/>
     </row>
-    <row r="4" spans="1:72" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="86"/>
-      <c r="C4" s="86"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="87"/>
-      <c r="F4" s="87"/>
-      <c r="G4" s="87"/>
-      <c r="H4" s="87"/>
-      <c r="I4" s="87"/>
-      <c r="J4" s="87"/>
-      <c r="K4" s="87"/>
+    <row r="4" spans="1:72" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="70"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
       <c r="L4" s="51" t="s">
         <v>109</v>
       </c>
       <c r="M4" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="N4" s="87"/>
-      <c r="O4" s="87"/>
-      <c r="P4" s="87"/>
-      <c r="Q4" s="87"/>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
-      <c r="T4" s="87"/>
-      <c r="U4" s="87"/>
-      <c r="V4" s="87"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="87"/>
-      <c r="AD4" s="87"/>
-      <c r="AE4" s="87"/>
-      <c r="AF4" s="87"/>
-      <c r="AG4" s="87"/>
-      <c r="AH4" s="87"/>
-      <c r="AI4" s="87"/>
-      <c r="AJ4" s="87"/>
-      <c r="AK4" s="87"/>
-      <c r="AL4" s="87"/>
-      <c r="AM4" s="87"/>
-      <c r="AN4" s="87"/>
-      <c r="AO4" s="87"/>
-      <c r="AP4" s="87"/>
-      <c r="AQ4" s="87"/>
-      <c r="AR4" s="87"/>
-      <c r="AS4" s="87"/>
-      <c r="AT4" s="87"/>
-      <c r="AU4" s="91"/>
-      <c r="AV4" s="87"/>
-      <c r="AW4" s="87"/>
-      <c r="AX4" s="89"/>
-      <c r="AY4" s="78" t="s">
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+      <c r="R4" s="69"/>
+      <c r="S4" s="69"/>
+      <c r="T4" s="69"/>
+      <c r="U4" s="69"/>
+      <c r="V4" s="69"/>
+      <c r="W4" s="69"/>
+      <c r="X4" s="69"/>
+      <c r="Y4" s="69"/>
+      <c r="Z4" s="69"/>
+      <c r="AA4" s="69"/>
+      <c r="AB4" s="69"/>
+      <c r="AC4" s="69"/>
+      <c r="AD4" s="69"/>
+      <c r="AE4" s="69"/>
+      <c r="AF4" s="69"/>
+      <c r="AG4" s="69"/>
+      <c r="AH4" s="69"/>
+      <c r="AI4" s="69"/>
+      <c r="AJ4" s="69"/>
+      <c r="AK4" s="69"/>
+      <c r="AL4" s="69"/>
+      <c r="AM4" s="69"/>
+      <c r="AN4" s="69"/>
+      <c r="AO4" s="69"/>
+      <c r="AP4" s="69"/>
+      <c r="AQ4" s="69"/>
+      <c r="AR4" s="69"/>
+      <c r="AS4" s="69"/>
+      <c r="AT4" s="69"/>
+      <c r="AU4" s="79"/>
+      <c r="AV4" s="69"/>
+      <c r="AW4" s="69"/>
+      <c r="AX4" s="77"/>
+      <c r="AY4" s="80" t="s">
         <v>176</v>
       </c>
-      <c r="AZ4" s="79"/>
-      <c r="BA4" s="79"/>
-      <c r="BB4" s="79"/>
-      <c r="BC4" s="79"/>
-      <c r="BD4" s="79"/>
-      <c r="BE4" s="79"/>
-      <c r="BF4" s="79"/>
-      <c r="BG4" s="77" t="s">
+      <c r="AZ4" s="81"/>
+      <c r="BA4" s="81"/>
+      <c r="BB4" s="81"/>
+      <c r="BC4" s="81"/>
+      <c r="BD4" s="81"/>
+      <c r="BE4" s="81"/>
+      <c r="BF4" s="81"/>
+      <c r="BG4" s="89" t="s">
         <v>177</v>
       </c>
-      <c r="BH4" s="77"/>
+      <c r="BH4" s="89"/>
       <c r="BI4" s="58" t="s">
         <v>204</v>
       </c>
       <c r="BJ4" s="58" t="s">
         <v>205</v>
       </c>
-      <c r="BK4" s="82" t="s">
+      <c r="BK4" s="85" t="s">
         <v>178</v>
       </c>
-      <c r="BL4" s="82"/>
-      <c r="BM4" s="82" t="s">
+      <c r="BL4" s="85"/>
+      <c r="BM4" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="BN4" s="82"/>
+      <c r="BN4" s="85"/>
       <c r="BO4" s="61" t="s">
         <v>180</v>
       </c>
@@ -2225,7 +2228,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="5" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A5" s="60"/>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
@@ -2340,74 +2343,74 @@
       <c r="AV5" s="51"/>
       <c r="AW5" s="51"/>
       <c r="AX5" s="52"/>
-      <c r="AY5" s="83" t="s">
+      <c r="AY5" s="86" t="s">
         <v>190</v>
       </c>
-      <c r="AZ5" s="84" t="s">
+      <c r="AZ5" s="87" t="s">
         <v>191</v>
       </c>
-      <c r="BA5" s="84" t="s">
+      <c r="BA5" s="87" t="s">
         <v>192</v>
       </c>
-      <c r="BB5" s="84" t="s">
+      <c r="BB5" s="87" t="s">
         <v>193</v>
       </c>
-      <c r="BC5" s="84" t="s">
+      <c r="BC5" s="87" t="s">
         <v>194</v>
       </c>
-      <c r="BD5" s="84" t="s">
+      <c r="BD5" s="87" t="s">
         <v>195</v>
       </c>
-      <c r="BE5" s="84" t="s">
+      <c r="BE5" s="87" t="s">
         <v>196</v>
       </c>
-      <c r="BF5" s="85" t="s">
+      <c r="BF5" s="88" t="s">
         <v>184</v>
       </c>
-      <c r="BG5" s="77" t="s">
+      <c r="BG5" s="89" t="s">
         <v>175</v>
       </c>
-      <c r="BH5" s="77" t="s">
+      <c r="BH5" s="89" t="s">
         <v>184</v>
       </c>
-      <c r="BI5" s="68" t="s">
+      <c r="BI5" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="BJ5" s="68" t="s">
+      <c r="BJ5" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="BK5" s="75" t="s">
+      <c r="BK5" s="97" t="s">
         <v>168</v>
       </c>
-      <c r="BL5" s="76" t="s">
+      <c r="BL5" s="84" t="s">
         <v>184</v>
       </c>
-      <c r="BM5" s="75" t="s">
+      <c r="BM5" s="97" t="s">
         <v>168</v>
       </c>
-      <c r="BN5" s="76" t="s">
+      <c r="BN5" s="84" t="s">
         <v>184</v>
       </c>
-      <c r="BO5" s="76" t="s">
+      <c r="BO5" s="84" t="s">
         <v>184</v>
       </c>
-      <c r="BP5" s="76" t="s">
+      <c r="BP5" s="84" t="s">
         <v>184</v>
       </c>
-      <c r="BQ5" s="68" t="s">
+      <c r="BQ5" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="BR5" s="68" t="s">
+      <c r="BR5" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="BS5" s="68" t="s">
+      <c r="BS5" s="90" t="s">
         <v>197</v>
       </c>
-      <c r="BT5" s="68" t="s">
+      <c r="BT5" s="90" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A6" s="51" t="s">
         <v>10</v>
       </c>
@@ -2558,30 +2561,30 @@
       <c r="AX6" s="52">
         <v>48</v>
       </c>
-      <c r="AY6" s="83"/>
-      <c r="AZ6" s="84"/>
-      <c r="BA6" s="84"/>
-      <c r="BB6" s="84"/>
-      <c r="BC6" s="84"/>
-      <c r="BD6" s="84"/>
-      <c r="BE6" s="84"/>
-      <c r="BF6" s="85"/>
-      <c r="BG6" s="77"/>
-      <c r="BH6" s="77"/>
-      <c r="BI6" s="68"/>
-      <c r="BJ6" s="68"/>
-      <c r="BK6" s="75"/>
-      <c r="BL6" s="76"/>
-      <c r="BM6" s="75"/>
-      <c r="BN6" s="76"/>
-      <c r="BO6" s="76"/>
-      <c r="BP6" s="76"/>
-      <c r="BQ6" s="68"/>
-      <c r="BR6" s="68"/>
-      <c r="BS6" s="68"/>
-      <c r="BT6" s="68"/>
+      <c r="AY6" s="86"/>
+      <c r="AZ6" s="87"/>
+      <c r="BA6" s="87"/>
+      <c r="BB6" s="87"/>
+      <c r="BC6" s="87"/>
+      <c r="BD6" s="87"/>
+      <c r="BE6" s="87"/>
+      <c r="BF6" s="88"/>
+      <c r="BG6" s="89"/>
+      <c r="BH6" s="89"/>
+      <c r="BI6" s="90"/>
+      <c r="BJ6" s="90"/>
+      <c r="BK6" s="97"/>
+      <c r="BL6" s="84"/>
+      <c r="BM6" s="97"/>
+      <c r="BN6" s="84"/>
+      <c r="BO6" s="84"/>
+      <c r="BP6" s="84"/>
+      <c r="BQ6" s="90"/>
+      <c r="BR6" s="90"/>
+      <c r="BS6" s="90"/>
+      <c r="BT6" s="90"/>
     </row>
-    <row r="7" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -2812,7 +2815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -3043,7 +3046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
@@ -3275,7 +3278,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>20</v>
       </c>
@@ -3507,7 +3510,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>22</v>
       </c>
@@ -3739,7 +3742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
@@ -3971,7 +3974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>26</v>
       </c>
@@ -4203,7 +4206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
@@ -4435,7 +4438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>30</v>
       </c>
@@ -4667,7 +4670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
@@ -4899,7 +4902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
@@ -5131,7 +5134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>36</v>
       </c>
@@ -5362,7 +5365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>38</v>
       </c>
@@ -5593,7 +5596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>40</v>
       </c>
@@ -5824,7 +5827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
@@ -6055,7 +6058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>44</v>
       </c>
@@ -6286,7 +6289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>46</v>
       </c>
@@ -6519,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>48</v>
       </c>
@@ -6750,7 +6753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>50</v>
       </c>
@@ -6981,7 +6984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>52</v>
       </c>
@@ -7212,7 +7215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>54</v>
       </c>
@@ -7443,7 +7446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>56</v>
       </c>
@@ -7670,7 +7673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>58</v>
       </c>
@@ -7897,7 +7900,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>60</v>
       </c>
@@ -8123,7 +8126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>62</v>
       </c>
@@ -8355,7 +8358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>63</v>
       </c>
@@ -8593,7 +8596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>64</v>
       </c>
@@ -8831,7 +8834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>65</v>
       </c>
@@ -9063,7 +9066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>149</v>
       </c>
@@ -9295,7 +9298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
         <v>150</v>
       </c>
@@ -9527,7 +9530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>68</v>
       </c>
@@ -9761,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>70</v>
       </c>
@@ -9995,7 +9998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
         <v>72</v>
       </c>
@@ -10229,7 +10232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>74</v>
       </c>
@@ -10462,7 +10465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>76</v>
       </c>
@@ -10717,7 +10720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>78</v>
       </c>
@@ -10972,7 +10975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>79</v>
       </c>
@@ -11227,7 +11230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:72" ht="24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:72" ht="24" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>80</v>
       </c>
@@ -11482,7 +11485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>81</v>
       </c>
@@ -11737,7 +11740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
         <v>82</v>
       </c>
@@ -11992,7 +11995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="30" t="s">
         <v>147</v>
       </c>
@@ -12247,8 +12250,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:72" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="69" t="s">
+    <row r="48" spans="1:72" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="91" t="s">
         <v>172</v>
       </c>
       <c r="B48" s="53" t="s">
@@ -12419,8 +12422,8 @@
       <c r="BS48" s="1"/>
       <c r="BT48" s="1"/>
     </row>
-    <row r="49" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A49" s="70"/>
+    <row r="49" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A49" s="92"/>
       <c r="B49" s="54" t="s">
         <v>185</v>
       </c>
@@ -12636,7 +12639,7 @@
       <c r="BS49" s="1"/>
       <c r="BT49" s="1"/>
     </row>
-    <row r="50" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A50" s="13"/>
       <c r="B50" s="59"/>
       <c r="C50" s="16"/>
@@ -12710,8 +12713,8 @@
       <c r="BS50" s="1"/>
       <c r="BT50" s="1"/>
     </row>
-    <row r="51" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A51" s="71" t="s">
+    <row r="51" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A51" s="93" t="s">
         <v>186</v>
       </c>
       <c r="B51" s="59" t="s">
@@ -12950,8 +12953,8 @@
       <c r="BS51" s="1"/>
       <c r="BT51" s="1"/>
     </row>
-    <row r="52" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A52" s="71"/>
+    <row r="52" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A52" s="93"/>
       <c r="B52" s="62" t="s">
         <v>187</v>
       </c>
@@ -13188,8 +13191,8 @@
       <c r="BS52" s="1"/>
       <c r="BT52" s="1"/>
     </row>
-    <row r="53" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A53" s="71"/>
+    <row r="53" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A53" s="93"/>
       <c r="B53" s="63"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
@@ -13262,8 +13265,8 @@
       <c r="BS53" s="1"/>
       <c r="BT53" s="1"/>
     </row>
-    <row r="54" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A54" s="71"/>
+    <row r="54" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A54" s="93"/>
       <c r="B54" s="59" t="s">
         <v>173</v>
       </c>
@@ -13500,8 +13503,8 @@
       <c r="BS54" s="1"/>
       <c r="BT54" s="1"/>
     </row>
-    <row r="55" spans="1:72" x14ac:dyDescent="0.25">
-      <c r="A55" s="71"/>
+    <row r="55" spans="1:72" x14ac:dyDescent="0.3">
+      <c r="A55" s="93"/>
       <c r="B55" s="62" t="s">
         <v>188</v>
       </c>
@@ -13738,7 +13741,7 @@
       <c r="BS55" s="1"/>
       <c r="BT55" s="1"/>
     </row>
-    <row r="56" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A56" s="2"/>
       <c r="B56" s="64"/>
       <c r="C56" s="2"/>
@@ -13812,7 +13815,7 @@
       <c r="BS56" s="1"/>
       <c r="BT56" s="1"/>
     </row>
-    <row r="57" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A57" s="2"/>
       <c r="B57" s="59" t="s">
         <v>198</v>
@@ -14050,7 +14053,7 @@
       <c r="BS57" s="1"/>
       <c r="BT57" s="1"/>
     </row>
-    <row r="58" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A58" s="2"/>
       <c r="B58" s="62" t="s">
         <v>199</v>
@@ -14288,7 +14291,7 @@
       <c r="BS58" s="1"/>
       <c r="BT58" s="1"/>
     </row>
-    <row r="59" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A59" s="2"/>
       <c r="B59" s="64"/>
       <c r="C59" s="2"/>
@@ -14362,7 +14365,7 @@
       <c r="BS59" s="1"/>
       <c r="BT59" s="1"/>
     </row>
-    <row r="60" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A60" s="2"/>
       <c r="B60" s="54" t="s">
         <v>201</v>
@@ -14600,7 +14603,7 @@
       <c r="BS60" s="1"/>
       <c r="BT60" s="1"/>
     </row>
-    <row r="61" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A61" s="2"/>
       <c r="B61" s="64"/>
       <c r="C61" s="2"/>
@@ -14674,7 +14677,7 @@
       <c r="BS61" s="1"/>
       <c r="BT61" s="1"/>
     </row>
-    <row r="62" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A62" s="2"/>
       <c r="B62" s="54" t="s">
         <v>202</v>
@@ -14912,7 +14915,7 @@
       <c r="BS62" s="1"/>
       <c r="BT62" s="1"/>
     </row>
-    <row r="63" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A63" s="2"/>
       <c r="B63" s="64"/>
       <c r="C63" s="2"/>
@@ -14986,7 +14989,7 @@
       <c r="BS63" s="1"/>
       <c r="BT63" s="1"/>
     </row>
-    <row r="64" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A64" s="2"/>
       <c r="B64" s="54" t="s">
         <v>203</v>
@@ -15224,7 +15227,7 @@
       <c r="BS64" s="1"/>
       <c r="BT64" s="1"/>
     </row>
-    <row r="65" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2"/>
       <c r="B65" s="64"/>
       <c r="C65" s="2"/>
@@ -15298,9 +15301,9 @@
       <c r="BS65" s="1"/>
       <c r="BT65" s="1"/>
     </row>
-    <row r="66" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A66" s="2"/>
-      <c r="B66" s="72" t="s">
+      <c r="B66" s="94" t="s">
         <v>206</v>
       </c>
       <c r="C66" s="39"/>
@@ -15512,9 +15515,9 @@
       <c r="BS66" s="1"/>
       <c r="BT66" s="1"/>
     </row>
-    <row r="67" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A67" s="2"/>
-      <c r="B67" s="73"/>
+      <c r="B67" s="95"/>
       <c r="C67" s="55"/>
       <c r="D67" s="38">
         <f>D37</f>
@@ -15724,9 +15727,9 @@
       <c r="BS67" s="1"/>
       <c r="BT67" s="1"/>
     </row>
-    <row r="68" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A68" s="2"/>
-      <c r="B68" s="73"/>
+      <c r="B68" s="95"/>
       <c r="C68" s="55"/>
       <c r="D68" s="38">
         <f>D38</f>
@@ -15939,9 +15942,9 @@
       <c r="BS68" s="1"/>
       <c r="BT68" s="1"/>
     </row>
-    <row r="69" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A69" s="2"/>
-      <c r="B69" s="73"/>
+      <c r="B69" s="95"/>
       <c r="C69" s="55"/>
       <c r="D69" s="38">
         <f>D39</f>
@@ -16154,9 +16157,9 @@
       <c r="BS69" s="1"/>
       <c r="BT69" s="1"/>
     </row>
-    <row r="70" spans="1:72" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:72" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
-      <c r="B70" s="74"/>
+      <c r="B70" s="96"/>
       <c r="C70" s="43"/>
       <c r="D70" s="43">
         <v>0</v>
@@ -16323,7 +16326,7 @@
       <c r="BS70" s="1"/>
       <c r="BT70" s="1"/>
     </row>
-    <row r="71" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A71" s="2"/>
       <c r="B71" s="64"/>
       <c r="C71" s="2"/>
@@ -16400,7 +16403,7 @@
       <c r="BS71" s="1"/>
       <c r="BT71" s="1"/>
     </row>
-    <row r="72" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A72" s="2"/>
       <c r="B72" s="65" t="s">
         <v>209</v>
@@ -16470,7 +16473,7 @@
       <c r="BS72" s="1"/>
       <c r="BT72" s="1"/>
     </row>
-    <row r="73" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A73" s="2"/>
       <c r="B73" s="65" t="s">
         <v>18</v>
@@ -16540,7 +16543,7 @@
       <c r="BS73" s="1"/>
       <c r="BT73" s="1"/>
     </row>
-    <row r="74" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A74" s="2"/>
       <c r="B74" s="65"/>
       <c r="C74" s="47"/>
@@ -16608,7 +16611,7 @@
       <c r="BS74" s="1"/>
       <c r="BT74" s="1"/>
     </row>
-    <row r="75" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A75" s="2"/>
       <c r="B75" s="65" t="s">
         <v>22</v>
@@ -16678,7 +16681,7 @@
       <c r="BS75" s="1"/>
       <c r="BT75" s="1"/>
     </row>
-    <row r="76" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A76" s="2"/>
       <c r="B76" s="65" t="s">
         <v>24</v>
@@ -16748,7 +16751,7 @@
       <c r="BS76" s="1"/>
       <c r="BT76" s="1"/>
     </row>
-    <row r="77" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A77" s="2"/>
       <c r="B77" s="65"/>
       <c r="C77" s="47"/>
@@ -16821,7 +16824,7 @@
       <c r="BS77" s="1"/>
       <c r="BT77" s="1"/>
     </row>
-    <row r="78" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A78" s="2"/>
       <c r="B78" s="65" t="s">
         <v>210</v>
@@ -16891,7 +16894,7 @@
       <c r="BS78" s="1"/>
       <c r="BT78" s="1"/>
     </row>
-    <row r="79" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A79" s="2"/>
       <c r="B79" s="65" t="s">
         <v>211</v>
@@ -16961,7 +16964,7 @@
       <c r="BS79" s="1"/>
       <c r="BT79" s="1"/>
     </row>
-    <row r="80" spans="1:72" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:72" x14ac:dyDescent="0.3">
       <c r="A80" s="2"/>
       <c r="B80" s="65" t="s">
         <v>212</v>
@@ -17033,26 +17036,61 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="K1:V1"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="N2:N4"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="R2:R4"/>
-    <mergeCell ref="S2:S4"/>
-    <mergeCell ref="T2:T4"/>
-    <mergeCell ref="U2:U4"/>
-    <mergeCell ref="V2:V4"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="D1:D4"/>
-    <mergeCell ref="E1:J1"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="F2:F4"/>
-    <mergeCell ref="G2:G4"/>
-    <mergeCell ref="H2:H4"/>
-    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="BT5:BT6"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="A51:A55"/>
+    <mergeCell ref="B66:B70"/>
+    <mergeCell ref="BM5:BM6"/>
+    <mergeCell ref="BN5:BN6"/>
+    <mergeCell ref="BO5:BO6"/>
+    <mergeCell ref="BP5:BP6"/>
+    <mergeCell ref="BQ5:BQ6"/>
+    <mergeCell ref="BR5:BR6"/>
+    <mergeCell ref="BG5:BG6"/>
+    <mergeCell ref="BH5:BH6"/>
+    <mergeCell ref="BI5:BI6"/>
+    <mergeCell ref="BJ5:BJ6"/>
+    <mergeCell ref="BK5:BK6"/>
+    <mergeCell ref="AY4:BF4"/>
+    <mergeCell ref="AY1:BS3"/>
+    <mergeCell ref="BL5:BL6"/>
+    <mergeCell ref="BK4:BL4"/>
+    <mergeCell ref="BM4:BN4"/>
+    <mergeCell ref="AY5:AY6"/>
+    <mergeCell ref="AZ5:AZ6"/>
+    <mergeCell ref="BA5:BA6"/>
+    <mergeCell ref="BB5:BB6"/>
+    <mergeCell ref="BC5:BC6"/>
+    <mergeCell ref="BD5:BD6"/>
+    <mergeCell ref="BE5:BE6"/>
+    <mergeCell ref="BF5:BF6"/>
+    <mergeCell ref="BG4:BH4"/>
+    <mergeCell ref="BS5:BS6"/>
+    <mergeCell ref="AR2:AR4"/>
+    <mergeCell ref="AS2:AV2"/>
+    <mergeCell ref="AW2:AW4"/>
+    <mergeCell ref="AX2:AX4"/>
+    <mergeCell ref="AP2:AP4"/>
+    <mergeCell ref="AQ2:AQ4"/>
+    <mergeCell ref="AS3:AS4"/>
+    <mergeCell ref="AT3:AT4"/>
+    <mergeCell ref="AU3:AU4"/>
+    <mergeCell ref="AV3:AV4"/>
+    <mergeCell ref="AM3:AM4"/>
+    <mergeCell ref="AG3:AG4"/>
+    <mergeCell ref="AH3:AH4"/>
+    <mergeCell ref="AI3:AI4"/>
+    <mergeCell ref="AK3:AK4"/>
+    <mergeCell ref="AL3:AL4"/>
+    <mergeCell ref="AE2:AI2"/>
+    <mergeCell ref="AE3:AE4"/>
+    <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:K4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="W2:W4"/>
     <mergeCell ref="W1:AI1"/>
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AN1:AQ1"/>
@@ -17069,61 +17107,26 @@
     <mergeCell ref="AK2:AM2"/>
     <mergeCell ref="AN2:AN4"/>
     <mergeCell ref="AO2:AO4"/>
-    <mergeCell ref="AE2:AI2"/>
-    <mergeCell ref="AE3:AE4"/>
-    <mergeCell ref="AF3:AF4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:K4"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="AM3:AM4"/>
-    <mergeCell ref="AG3:AG4"/>
-    <mergeCell ref="AH3:AH4"/>
-    <mergeCell ref="AI3:AI4"/>
-    <mergeCell ref="AK3:AK4"/>
-    <mergeCell ref="AL3:AL4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="AR2:AR4"/>
-    <mergeCell ref="AS2:AV2"/>
-    <mergeCell ref="AW2:AW4"/>
-    <mergeCell ref="AX2:AX4"/>
-    <mergeCell ref="AP2:AP4"/>
-    <mergeCell ref="AQ2:AQ4"/>
-    <mergeCell ref="AS3:AS4"/>
-    <mergeCell ref="AT3:AT4"/>
-    <mergeCell ref="AU3:AU4"/>
-    <mergeCell ref="AV3:AV4"/>
-    <mergeCell ref="AY4:BF4"/>
-    <mergeCell ref="AY1:BS3"/>
-    <mergeCell ref="BL5:BL6"/>
-    <mergeCell ref="BK4:BL4"/>
-    <mergeCell ref="BM4:BN4"/>
-    <mergeCell ref="AY5:AY6"/>
-    <mergeCell ref="AZ5:AZ6"/>
-    <mergeCell ref="BA5:BA6"/>
-    <mergeCell ref="BB5:BB6"/>
-    <mergeCell ref="BC5:BC6"/>
-    <mergeCell ref="BD5:BD6"/>
-    <mergeCell ref="BE5:BE6"/>
-    <mergeCell ref="BF5:BF6"/>
-    <mergeCell ref="BG4:BH4"/>
-    <mergeCell ref="BS5:BS6"/>
-    <mergeCell ref="BT5:BT6"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="B66:B70"/>
-    <mergeCell ref="BM5:BM6"/>
-    <mergeCell ref="BN5:BN6"/>
-    <mergeCell ref="BO5:BO6"/>
-    <mergeCell ref="BP5:BP6"/>
-    <mergeCell ref="BQ5:BQ6"/>
-    <mergeCell ref="BR5:BR6"/>
-    <mergeCell ref="BG5:BG6"/>
-    <mergeCell ref="BH5:BH6"/>
-    <mergeCell ref="BI5:BI6"/>
-    <mergeCell ref="BJ5:BJ6"/>
-    <mergeCell ref="BK5:BK6"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:J1"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
+    <mergeCell ref="G2:G4"/>
+    <mergeCell ref="H2:H4"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="K1:V1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="N2:N4"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="R2:R4"/>
+    <mergeCell ref="S2:S4"/>
+    <mergeCell ref="T2:T4"/>
+    <mergeCell ref="U2:U4"/>
+    <mergeCell ref="V2:V4"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C47">
     <cfRule type="cellIs" dxfId="6" priority="26" stopIfTrue="1" operator="equal">

</xml_diff>